<commit_message>
20201126 CRE20-015-06	Special Support Scheme for Continuing Medical Care to HA Patients in GD (SSSCMC) – Phase 6 20201127 CRE20-014-02	To add new seasonal influenza vaccine under VSS and PPP-KG with subsidy at $100 per dose - Phase 2 20201127 CRE20-015-07	Special Support Scheme for Continuing Medical Care to HA Patients in GD (SSSCMC) - Phase 7 20201127 CRE20-016	To update the format of the Pre Authorization Checking File 20201127 CRS20-027	To update the English name of a school recorded on eHS(S) for subsequent batch upload/claim/reimbursement process under the SIVOP 2020/21 20201127 CRS20-028	Patch Subsidy of PPPKG Vaccination File
</commit_message>
<xml_diff>
--- a/EHS2019/EHS/ExcelGenerator/Template/eHSD0033-PPPKG Claim_Template.xlsx
+++ b/EHS2019/EHS/ExcelGenerator/Template/eHSD0033-PPPKG Claim_Template.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Project\EHS2019_BatchUpload\ExcelGenerator\bin\Debug\Template\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\ce5-fs01\ehs$\Development\InternalChangeControl\2020\CRE20-0XX (Gov SIV 2020_21)\Front-end (Phase 2)\ExcelGenerator\Template\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="930" yWindow="1290" windowWidth="18570" windowHeight="7500" tabRatio="760"/>
+    <workbookView xWindow="930" yWindow="1290" windowWidth="18570" windowHeight="7500" tabRatio="820"/>
   </bookViews>
   <sheets>
     <sheet name="Content" sheetId="24" r:id="rId1"/>
@@ -17,16 +17,18 @@
     <sheet name="02-Age Group" sheetId="22" r:id="rId3"/>
     <sheet name="03-QIV" sheetId="28" r:id="rId4"/>
     <sheet name="03-LAIV" sheetId="29" r:id="rId5"/>
-    <sheet name="04-Raw Data" sheetId="23" r:id="rId6"/>
-    <sheet name="Remark" sheetId="6" r:id="rId7"/>
-    <sheet name="Change History" sheetId="25" r:id="rId8"/>
+    <sheet name="03-QIV (Govt)" sheetId="30" r:id="rId6"/>
+    <sheet name="03-LAIV (Govt)" sheetId="31" r:id="rId7"/>
+    <sheet name="04-Raw Data" sheetId="23" r:id="rId8"/>
+    <sheet name="Remark" sheetId="6" r:id="rId9"/>
+    <sheet name="Change History" sheetId="25" r:id="rId10"/>
   </sheets>
-  <calcPr calcId="152511"/>
+  <calcPr calcId="162913"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="275" uniqueCount="85">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="311" uniqueCount="87">
   <si>
     <t/>
   </si>
@@ -333,12 +335,20 @@
   </si>
   <si>
     <t>CRE19-001</t>
+  </si>
+  <si>
+    <t>CRE20-014</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>To add new seasonal influenza vaccine under VSS and PPP-KG with subsidy at $100 per dose</t>
+    <phoneticPr fontId="3" type="noConversion"/>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <numFmts count="3">
     <numFmt numFmtId="176" formatCode="yyyy/mm/dd"/>
     <numFmt numFmtId="177" formatCode="yyyy/mm/dd\ hh:mm:ss"/>
@@ -1068,7 +1078,9 @@
   </sheetPr>
   <dimension ref="A1:B8"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A6" sqref="A6"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
@@ -1133,6 +1145,87 @@
   <phoneticPr fontId="3" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup paperSize="9" orientation="landscape" r:id="rId1"/>
+  <headerFooter alignWithMargins="0"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:D5"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="8.5" style="44" customWidth="1"/>
+    <col min="2" max="2" width="14.375" style="44" customWidth="1"/>
+    <col min="3" max="3" width="84.875" style="44" customWidth="1"/>
+    <col min="4" max="4" width="15.625" style="44" customWidth="1"/>
+    <col min="5" max="16384" width="9" style="44"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="11" t="s">
+        <v>33</v>
+      </c>
+      <c r="B1" s="1"/>
+      <c r="C1" s="1"/>
+      <c r="D1" s="1"/>
+    </row>
+    <row r="2" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="1"/>
+      <c r="B2" s="1"/>
+      <c r="C2" s="1"/>
+      <c r="D2" s="1"/>
+    </row>
+    <row r="3" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="D3" s="2" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A4" s="88">
+        <v>1</v>
+      </c>
+      <c r="B4" s="88" t="s">
+        <v>84</v>
+      </c>
+      <c r="C4" s="100" t="s">
+        <v>74</v>
+      </c>
+      <c r="D4" s="104">
+        <v>43747</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="A5" s="88">
+        <v>2</v>
+      </c>
+      <c r="B5" s="88" t="s">
+        <v>85</v>
+      </c>
+      <c r="C5" s="100" t="s">
+        <v>86</v>
+      </c>
+      <c r="D5" s="104">
+        <v>44151</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="3" type="noConversion"/>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
   <headerFooter alignWithMargins="0"/>
 </worksheet>
 </file>
@@ -1847,17 +1940,20 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:AB23"/>
+  <dimension ref="A1:AB29"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="18.625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="22.375" style="88" customWidth="1"/>
-    <col min="2" max="16384" width="18.625" style="88"/>
+    <col min="2" max="2" width="21.625" style="88" customWidth="1"/>
+    <col min="3" max="3" width="18.625" style="88"/>
+    <col min="4" max="4" width="23.5" style="88" customWidth="1"/>
+    <col min="5" max="16384" width="18.625" style="88"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:28" s="85" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" s="85" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="15" t="str">
         <f>Content!A3 &amp; ": " &amp;Content!B3</f>
         <v>eHS(S)D0033-02: Report on yearly PPP-KG claim transaction by age group and target group (YYYY/YY)</v>
@@ -1868,7 +1964,7 @@
       <c r="E1" s="101"/>
       <c r="F1" s="102"/>
     </row>
-    <row r="2" spans="1:28" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="97"/>
       <c r="B2" s="81"/>
       <c r="C2" s="98"/>
@@ -1876,7 +1972,7 @@
       <c r="E2" s="98"/>
       <c r="F2" s="55"/>
     </row>
-    <row r="3" spans="1:28" s="85" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:9" s="85" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="57" t="s">
         <v>38</v>
       </c>
@@ -1886,10 +1982,10 @@
       <c r="E3" s="101"/>
       <c r="F3" s="102"/>
     </row>
-    <row r="4" spans="1:28" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="80"/>
     </row>
-    <row r="5" spans="1:28" s="8" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:9" s="8" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="62" t="s">
         <v>60</v>
       </c>
@@ -1902,7 +1998,7 @@
       <c r="H5" s="85"/>
       <c r="I5" s="75"/>
     </row>
-    <row r="6" spans="1:28" s="49" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:9" s="49" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="82"/>
       <c r="B6" s="79"/>
       <c r="C6" s="65"/>
@@ -1912,11 +2008,14 @@
       <c r="H6" s="88"/>
       <c r="I6" s="65"/>
     </row>
-    <row r="7" spans="1:28" s="8" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:9" s="8" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="67" t="s">
         <v>25</v>
       </c>
       <c r="B7" s="67" t="s">
+        <v>25</v>
+      </c>
+      <c r="C7" s="67" t="s">
         <v>25</v>
       </c>
       <c r="D7" s="75" t="s">
@@ -1928,387 +2027,218 @@
       <c r="H7" s="85"/>
       <c r="I7" s="61"/>
     </row>
-    <row r="8" spans="1:28" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="79" t="s">
         <v>39</v>
       </c>
       <c r="B8" s="79" t="s">
         <v>26</v>
       </c>
+      <c r="C8" s="79" t="s">
+        <v>26</v>
+      </c>
       <c r="D8" s="79" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="9" spans="1:28" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="79"/>
+    <row r="9" spans="1:9" s="49" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="82"/>
       <c r="B9" s="79"/>
-      <c r="C9" s="79"/>
-      <c r="D9" s="79"/>
-      <c r="E9" s="79"/>
-    </row>
-    <row r="11" spans="1:28" s="85" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="74" t="s">
+      <c r="C9" s="65"/>
+      <c r="D9" s="65"/>
+      <c r="F9" s="82"/>
+      <c r="G9" s="88"/>
+      <c r="H9" s="88"/>
+      <c r="I9" s="65"/>
+    </row>
+    <row r="10" spans="1:9" s="8" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="67" t="s">
+        <v>25</v>
+      </c>
+      <c r="B10" s="67" t="s">
+        <v>25</v>
+      </c>
+      <c r="C10" s="67" t="s">
+        <v>25</v>
+      </c>
+      <c r="D10" s="75" t="s">
+        <v>41</v>
+      </c>
+      <c r="E10" s="61"/>
+      <c r="F10" s="61"/>
+      <c r="G10" s="85"/>
+      <c r="H10" s="85"/>
+      <c r="I10" s="61"/>
+    </row>
+    <row r="11" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="79" t="s">
+        <v>39</v>
+      </c>
+      <c r="B11" s="79" t="s">
+        <v>26</v>
+      </c>
+      <c r="C11" s="79" t="s">
+        <v>26</v>
+      </c>
+      <c r="D11" s="79" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" s="49" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A12" s="82"/>
+      <c r="B12" s="79"/>
+      <c r="C12" s="65"/>
+      <c r="D12" s="65"/>
+      <c r="F12" s="82"/>
+      <c r="G12" s="88"/>
+      <c r="H12" s="88"/>
+      <c r="I12" s="65"/>
+    </row>
+    <row r="13" spans="1:9" s="8" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A13" s="67" t="s">
+        <v>25</v>
+      </c>
+      <c r="B13" s="67" t="s">
+        <v>25</v>
+      </c>
+      <c r="C13" s="67" t="s">
+        <v>25</v>
+      </c>
+      <c r="D13" s="75" t="s">
+        <v>41</v>
+      </c>
+      <c r="E13" s="61"/>
+      <c r="F13" s="61"/>
+      <c r="G13" s="85"/>
+      <c r="H13" s="85"/>
+      <c r="I13" s="61"/>
+    </row>
+    <row r="14" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A14" s="79" t="s">
+        <v>39</v>
+      </c>
+      <c r="B14" s="79" t="s">
+        <v>26</v>
+      </c>
+      <c r="C14" s="79" t="s">
+        <v>26</v>
+      </c>
+      <c r="D14" s="79" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A15" s="79"/>
+      <c r="B15" s="79"/>
+      <c r="C15" s="79"/>
+      <c r="D15" s="79"/>
+      <c r="E15" s="79"/>
+    </row>
+    <row r="17" spans="1:28" s="85" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A17" s="74" t="s">
         <v>61</v>
       </c>
     </row>
-    <row r="12" spans="1:28" s="68" customFormat="1" ht="33" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B12" s="66" t="s">
+    <row r="18" spans="1:28" s="68" customFormat="1" ht="33" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B18" s="66" t="s">
         <v>37</v>
       </c>
-      <c r="C12" s="75" t="s">
+      <c r="C18" s="75" t="s">
         <v>37</v>
       </c>
-      <c r="D12" s="75" t="s">
+      <c r="D18" s="75" t="s">
         <v>37</v>
       </c>
-      <c r="E12" s="75" t="s">
+      <c r="E18" s="75" t="s">
         <v>48</v>
       </c>
-      <c r="F12" s="75" t="s">
+      <c r="F18" s="75" t="s">
         <v>48</v>
       </c>
-      <c r="G12" s="75" t="s">
+      <c r="G18" s="75" t="s">
         <v>48</v>
       </c>
-      <c r="H12" s="68" t="s">
+      <c r="H18" s="68" t="s">
         <v>49</v>
       </c>
-      <c r="I12" s="68" t="s">
+      <c r="I18" s="68" t="s">
         <v>68</v>
       </c>
-      <c r="J12" s="77" t="s">
+      <c r="J18" s="77" t="s">
         <v>51</v>
       </c>
-      <c r="P12" s="69"/>
-      <c r="Q12" s="69"/>
-      <c r="R12" s="69"/>
-      <c r="S12" s="69"/>
-      <c r="T12" s="69"/>
-      <c r="U12" s="69"/>
-      <c r="V12" s="75"/>
-      <c r="W12" s="75"/>
-      <c r="X12" s="75"/>
-      <c r="Y12" s="75"/>
-      <c r="Z12" s="75"/>
-      <c r="AA12" s="75"/>
-      <c r="AB12" s="77"/>
-    </row>
-    <row r="13" spans="1:28" s="84" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="68"/>
-      <c r="B13" s="84" t="s">
+      <c r="P18" s="69"/>
+      <c r="Q18" s="69"/>
+      <c r="R18" s="69"/>
+      <c r="S18" s="69"/>
+      <c r="T18" s="69"/>
+      <c r="U18" s="69"/>
+      <c r="V18" s="75"/>
+      <c r="W18" s="75"/>
+      <c r="X18" s="75"/>
+      <c r="Y18" s="75"/>
+      <c r="Z18" s="75"/>
+      <c r="AA18" s="75"/>
+      <c r="AB18" s="77"/>
+    </row>
+    <row r="19" spans="1:28" s="84" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A19" s="68"/>
+      <c r="B19" s="84" t="s">
         <v>42</v>
       </c>
-      <c r="C13" s="84" t="s">
+      <c r="C19" s="84" t="s">
         <v>43</v>
       </c>
-      <c r="D13" s="84" t="s">
+      <c r="D19" s="84" t="s">
         <v>44</v>
       </c>
-      <c r="E13" s="84" t="s">
+      <c r="E19" s="84" t="s">
         <v>45</v>
       </c>
-      <c r="F13" s="84" t="s">
+      <c r="F19" s="84" t="s">
         <v>46</v>
       </c>
-      <c r="G13" s="84" t="s">
+      <c r="G19" s="84" t="s">
         <v>47</v>
       </c>
-      <c r="H13" s="84" t="s">
+      <c r="H19" s="84" t="s">
         <v>47</v>
       </c>
-      <c r="I13" s="84" t="s">
+      <c r="I19" s="84" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="14" spans="1:28" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="49" t="s">
+    <row r="20" spans="1:28" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A20" s="49" t="s">
         <v>40</v>
       </c>
-      <c r="B14" s="83" t="s">
+      <c r="B20" s="83" t="s">
         <v>40</v>
       </c>
-      <c r="C14" s="83" t="s">
+      <c r="C20" s="83" t="s">
         <v>40</v>
       </c>
-      <c r="D14" s="83" t="s">
+      <c r="D20" s="83" t="s">
         <v>40</v>
       </c>
-      <c r="E14" s="83" t="s">
+      <c r="E20" s="83" t="s">
         <v>40</v>
       </c>
-      <c r="F14" s="83" t="s">
+      <c r="F20" s="83" t="s">
         <v>40</v>
       </c>
-      <c r="G14" s="83" t="s">
+      <c r="G20" s="83" t="s">
         <v>40</v>
       </c>
-      <c r="H14" s="83" t="s">
+      <c r="H20" s="83" t="s">
         <v>40</v>
       </c>
-      <c r="I14" s="83" t="s">
+      <c r="I20" s="83" t="s">
         <v>40</v>
       </c>
-      <c r="J14" s="83" t="s">
+      <c r="J20" s="83" t="s">
         <v>40</v>
       </c>
-      <c r="K14" s="83"/>
-      <c r="L14" s="83"/>
-      <c r="M14" s="83"/>
-      <c r="N14" s="83"/>
-      <c r="O14" s="83"/>
-      <c r="P14" s="83"/>
-      <c r="Q14" s="83"/>
-      <c r="R14" s="83"/>
-      <c r="S14" s="83"/>
-      <c r="T14" s="83"/>
-      <c r="U14" s="83"/>
-      <c r="V14" s="83"/>
-      <c r="W14" s="83"/>
-      <c r="X14" s="83"/>
-      <c r="Y14" s="83"/>
-      <c r="Z14" s="83"/>
-      <c r="AA14" s="83"/>
-      <c r="AB14" s="83"/>
-    </row>
-    <row r="15" spans="1:28" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="49" t="s">
-        <v>26</v>
-      </c>
-      <c r="B15" s="83" t="s">
-        <v>26</v>
-      </c>
-      <c r="C15" s="83" t="s">
-        <v>26</v>
-      </c>
-      <c r="D15" s="83" t="s">
-        <v>26</v>
-      </c>
-      <c r="E15" s="83" t="s">
-        <v>26</v>
-      </c>
-      <c r="F15" s="83" t="s">
-        <v>26</v>
-      </c>
-      <c r="G15" s="83" t="s">
-        <v>26</v>
-      </c>
-      <c r="H15" s="83" t="s">
-        <v>26</v>
-      </c>
-      <c r="I15" s="83" t="s">
-        <v>26</v>
-      </c>
-      <c r="J15" s="83" t="s">
-        <v>26</v>
-      </c>
-      <c r="K15" s="83"/>
-      <c r="L15" s="83"/>
-      <c r="M15" s="83"/>
-      <c r="N15" s="83"/>
-      <c r="O15" s="83"/>
-      <c r="P15" s="83"/>
-      <c r="Q15" s="83"/>
-      <c r="R15" s="83"/>
-      <c r="S15" s="83"/>
-      <c r="T15" s="83"/>
-      <c r="U15" s="83"/>
-      <c r="V15" s="83"/>
-      <c r="W15" s="83"/>
-      <c r="X15" s="83"/>
-      <c r="Y15" s="83"/>
-      <c r="Z15" s="83"/>
-      <c r="AA15" s="83"/>
-      <c r="AB15" s="83"/>
-    </row>
-    <row r="16" spans="1:28" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="49" t="s">
-        <v>39</v>
-      </c>
-      <c r="B16" s="83" t="s">
-        <v>39</v>
-      </c>
-      <c r="C16" s="83" t="s">
-        <v>39</v>
-      </c>
-      <c r="D16" s="83" t="s">
-        <v>39</v>
-      </c>
-      <c r="E16" s="83" t="s">
-        <v>39</v>
-      </c>
-      <c r="F16" s="83" t="s">
-        <v>39</v>
-      </c>
-      <c r="G16" s="83" t="s">
-        <v>39</v>
-      </c>
-      <c r="H16" s="83" t="s">
-        <v>39</v>
-      </c>
-      <c r="I16" s="83" t="s">
-        <v>39</v>
-      </c>
-      <c r="J16" s="83" t="s">
-        <v>39</v>
-      </c>
-      <c r="K16" s="83"/>
-      <c r="L16" s="83"/>
-      <c r="M16" s="83"/>
-      <c r="N16" s="83"/>
-      <c r="O16" s="83"/>
-      <c r="P16" s="83"/>
-      <c r="Q16" s="83"/>
-      <c r="R16" s="83"/>
-      <c r="S16" s="83"/>
-      <c r="T16" s="83"/>
-      <c r="U16" s="83"/>
-      <c r="V16" s="83"/>
-      <c r="W16" s="83"/>
-      <c r="X16" s="83"/>
-      <c r="Y16" s="83"/>
-      <c r="Z16" s="83"/>
-      <c r="AA16" s="83"/>
-      <c r="AB16" s="83"/>
-    </row>
-    <row r="17" spans="1:28" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="49" t="s">
-        <v>26</v>
-      </c>
-      <c r="B17" s="83" t="s">
-        <v>26</v>
-      </c>
-      <c r="C17" s="83" t="s">
-        <v>26</v>
-      </c>
-      <c r="D17" s="83" t="s">
-        <v>26</v>
-      </c>
-      <c r="E17" s="83" t="s">
-        <v>26</v>
-      </c>
-      <c r="F17" s="83" t="s">
-        <v>26</v>
-      </c>
-      <c r="G17" s="83" t="s">
-        <v>26</v>
-      </c>
-      <c r="H17" s="83" t="s">
-        <v>26</v>
-      </c>
-      <c r="I17" s="83" t="s">
-        <v>26</v>
-      </c>
-      <c r="J17" s="83" t="s">
-        <v>26</v>
-      </c>
-      <c r="K17" s="83"/>
-      <c r="L17" s="83"/>
-      <c r="M17" s="83"/>
-      <c r="N17" s="83"/>
-      <c r="O17" s="83"/>
-      <c r="P17" s="83"/>
-      <c r="Q17" s="83"/>
-      <c r="R17" s="83"/>
-      <c r="S17" s="83"/>
-      <c r="T17" s="83"/>
-      <c r="U17" s="83"/>
-      <c r="V17" s="83"/>
-      <c r="W17" s="83"/>
-      <c r="X17" s="83"/>
-      <c r="Y17" s="83"/>
-      <c r="Z17" s="83"/>
-      <c r="AA17" s="83"/>
-      <c r="AB17" s="83"/>
-    </row>
-    <row r="18" spans="1:28" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B18" s="83"/>
-      <c r="C18" s="83"/>
-      <c r="D18" s="83"/>
-      <c r="E18" s="83"/>
-      <c r="F18" s="83"/>
-      <c r="G18" s="83"/>
-      <c r="H18" s="83"/>
-      <c r="I18" s="83"/>
-      <c r="J18" s="83"/>
-      <c r="K18" s="83"/>
-      <c r="L18" s="83"/>
-      <c r="M18" s="83"/>
-      <c r="N18" s="83"/>
-      <c r="O18" s="83"/>
-      <c r="P18" s="83"/>
-      <c r="Q18" s="83"/>
-      <c r="R18" s="83"/>
-      <c r="S18" s="83"/>
-      <c r="T18" s="83"/>
-      <c r="U18" s="83"/>
-      <c r="V18" s="83"/>
-      <c r="W18" s="83"/>
-      <c r="X18" s="83"/>
-      <c r="Y18" s="83"/>
-      <c r="Z18" s="83"/>
-      <c r="AA18" s="83"/>
-      <c r="AB18" s="83"/>
-    </row>
-    <row r="19" spans="1:28" s="85" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="85" t="s">
-        <v>83</v>
-      </c>
-      <c r="B19" s="73" t="s">
-        <v>40</v>
-      </c>
-      <c r="C19" s="73" t="s">
-        <v>40</v>
-      </c>
-      <c r="D19" s="73" t="s">
-        <v>40</v>
-      </c>
-      <c r="E19" s="73" t="s">
-        <v>40</v>
-      </c>
-      <c r="F19" s="73" t="s">
-        <v>40</v>
-      </c>
-      <c r="G19" s="73" t="s">
-        <v>40</v>
-      </c>
-      <c r="H19" s="73" t="s">
-        <v>40</v>
-      </c>
-      <c r="I19" s="73" t="s">
-        <v>40</v>
-      </c>
-      <c r="J19" s="73" t="s">
-        <v>40</v>
-      </c>
-      <c r="K19" s="73"/>
-      <c r="L19" s="73"/>
-      <c r="M19" s="73"/>
-      <c r="N19" s="73"/>
-      <c r="O19" s="73"/>
-      <c r="P19" s="73"/>
-      <c r="Q19" s="73"/>
-      <c r="R19" s="73"/>
-      <c r="S19" s="73"/>
-      <c r="T19" s="73"/>
-      <c r="U19" s="73"/>
-      <c r="V19" s="73"/>
-      <c r="W19" s="73"/>
-      <c r="X19" s="73"/>
-      <c r="Y19" s="73"/>
-      <c r="Z19" s="73"/>
-      <c r="AA19" s="73"/>
-      <c r="AB19" s="73"/>
-    </row>
-    <row r="20" spans="1:28" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B20" s="83"/>
-      <c r="C20" s="83"/>
-      <c r="D20" s="83"/>
-      <c r="E20" s="83"/>
-      <c r="F20" s="83"/>
-      <c r="G20" s="83"/>
-      <c r="H20" s="83"/>
-      <c r="I20" s="83"/>
-      <c r="J20" s="83"/>
       <c r="K20" s="83"/>
       <c r="L20" s="83"/>
       <c r="M20" s="83"/>
@@ -2329,25 +2259,283 @@
       <c r="AB20" s="83"/>
     </row>
     <row r="21" spans="1:28" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="F21" s="65"/>
-      <c r="G21" s="99"/>
+      <c r="A21" s="49" t="s">
+        <v>26</v>
+      </c>
+      <c r="B21" s="83" t="s">
+        <v>26</v>
+      </c>
+      <c r="C21" s="83" t="s">
+        <v>26</v>
+      </c>
+      <c r="D21" s="83" t="s">
+        <v>26</v>
+      </c>
+      <c r="E21" s="83" t="s">
+        <v>26</v>
+      </c>
+      <c r="F21" s="83" t="s">
+        <v>26</v>
+      </c>
+      <c r="G21" s="83" t="s">
+        <v>26</v>
+      </c>
+      <c r="H21" s="83" t="s">
+        <v>26</v>
+      </c>
+      <c r="I21" s="83" t="s">
+        <v>26</v>
+      </c>
+      <c r="J21" s="83" t="s">
+        <v>26</v>
+      </c>
+      <c r="K21" s="83"/>
+      <c r="L21" s="83"/>
+      <c r="M21" s="83"/>
+      <c r="N21" s="83"/>
+      <c r="O21" s="83"/>
+      <c r="P21" s="83"/>
+      <c r="Q21" s="83"/>
+      <c r="R21" s="83"/>
+      <c r="S21" s="83"/>
+      <c r="T21" s="83"/>
+      <c r="U21" s="83"/>
+      <c r="V21" s="83"/>
+      <c r="W21" s="83"/>
+      <c r="X21" s="83"/>
+      <c r="Y21" s="83"/>
+      <c r="Z21" s="83"/>
+      <c r="AA21" s="83"/>
+      <c r="AB21" s="83"/>
     </row>
     <row r="22" spans="1:28" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A22" s="85" t="s">
+      <c r="A22" s="49" t="s">
+        <v>39</v>
+      </c>
+      <c r="B22" s="83" t="s">
+        <v>39</v>
+      </c>
+      <c r="C22" s="83" t="s">
+        <v>39</v>
+      </c>
+      <c r="D22" s="83" t="s">
+        <v>39</v>
+      </c>
+      <c r="E22" s="83" t="s">
+        <v>39</v>
+      </c>
+      <c r="F22" s="83" t="s">
+        <v>39</v>
+      </c>
+      <c r="G22" s="83" t="s">
+        <v>39</v>
+      </c>
+      <c r="H22" s="83" t="s">
+        <v>39</v>
+      </c>
+      <c r="I22" s="83" t="s">
+        <v>39</v>
+      </c>
+      <c r="J22" s="83" t="s">
+        <v>39</v>
+      </c>
+      <c r="K22" s="83"/>
+      <c r="L22" s="83"/>
+      <c r="M22" s="83"/>
+      <c r="N22" s="83"/>
+      <c r="O22" s="83"/>
+      <c r="P22" s="83"/>
+      <c r="Q22" s="83"/>
+      <c r="R22" s="83"/>
+      <c r="S22" s="83"/>
+      <c r="T22" s="83"/>
+      <c r="U22" s="83"/>
+      <c r="V22" s="83"/>
+      <c r="W22" s="83"/>
+      <c r="X22" s="83"/>
+      <c r="Y22" s="83"/>
+      <c r="Z22" s="83"/>
+      <c r="AA22" s="83"/>
+      <c r="AB22" s="83"/>
+    </row>
+    <row r="23" spans="1:28" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A23" s="49" t="s">
+        <v>26</v>
+      </c>
+      <c r="B23" s="83" t="s">
+        <v>26</v>
+      </c>
+      <c r="C23" s="83" t="s">
+        <v>26</v>
+      </c>
+      <c r="D23" s="83" t="s">
+        <v>26</v>
+      </c>
+      <c r="E23" s="83" t="s">
+        <v>26</v>
+      </c>
+      <c r="F23" s="83" t="s">
+        <v>26</v>
+      </c>
+      <c r="G23" s="83" t="s">
+        <v>26</v>
+      </c>
+      <c r="H23" s="83" t="s">
+        <v>26</v>
+      </c>
+      <c r="I23" s="83" t="s">
+        <v>26</v>
+      </c>
+      <c r="J23" s="83" t="s">
+        <v>26</v>
+      </c>
+      <c r="K23" s="83"/>
+      <c r="L23" s="83"/>
+      <c r="M23" s="83"/>
+      <c r="N23" s="83"/>
+      <c r="O23" s="83"/>
+      <c r="P23" s="83"/>
+      <c r="Q23" s="83"/>
+      <c r="R23" s="83"/>
+      <c r="S23" s="83"/>
+      <c r="T23" s="83"/>
+      <c r="U23" s="83"/>
+      <c r="V23" s="83"/>
+      <c r="W23" s="83"/>
+      <c r="X23" s="83"/>
+      <c r="Y23" s="83"/>
+      <c r="Z23" s="83"/>
+      <c r="AA23" s="83"/>
+      <c r="AB23" s="83"/>
+    </row>
+    <row r="24" spans="1:28" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B24" s="83"/>
+      <c r="C24" s="83"/>
+      <c r="D24" s="83"/>
+      <c r="E24" s="83"/>
+      <c r="F24" s="83"/>
+      <c r="G24" s="83"/>
+      <c r="H24" s="83"/>
+      <c r="I24" s="83"/>
+      <c r="J24" s="83"/>
+      <c r="K24" s="83"/>
+      <c r="L24" s="83"/>
+      <c r="M24" s="83"/>
+      <c r="N24" s="83"/>
+      <c r="O24" s="83"/>
+      <c r="P24" s="83"/>
+      <c r="Q24" s="83"/>
+      <c r="R24" s="83"/>
+      <c r="S24" s="83"/>
+      <c r="T24" s="83"/>
+      <c r="U24" s="83"/>
+      <c r="V24" s="83"/>
+      <c r="W24" s="83"/>
+      <c r="X24" s="83"/>
+      <c r="Y24" s="83"/>
+      <c r="Z24" s="83"/>
+      <c r="AA24" s="83"/>
+      <c r="AB24" s="83"/>
+    </row>
+    <row r="25" spans="1:28" s="85" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A25" s="85" t="s">
+        <v>83</v>
+      </c>
+      <c r="B25" s="73" t="s">
+        <v>40</v>
+      </c>
+      <c r="C25" s="73" t="s">
+        <v>40</v>
+      </c>
+      <c r="D25" s="73" t="s">
+        <v>40</v>
+      </c>
+      <c r="E25" s="73" t="s">
+        <v>40</v>
+      </c>
+      <c r="F25" s="73" t="s">
+        <v>40</v>
+      </c>
+      <c r="G25" s="73" t="s">
+        <v>40</v>
+      </c>
+      <c r="H25" s="73" t="s">
+        <v>40</v>
+      </c>
+      <c r="I25" s="73" t="s">
+        <v>40</v>
+      </c>
+      <c r="J25" s="73" t="s">
+        <v>40</v>
+      </c>
+      <c r="K25" s="73"/>
+      <c r="L25" s="73"/>
+      <c r="M25" s="73"/>
+      <c r="N25" s="73"/>
+      <c r="O25" s="73"/>
+      <c r="P25" s="73"/>
+      <c r="Q25" s="73"/>
+      <c r="R25" s="73"/>
+      <c r="S25" s="73"/>
+      <c r="T25" s="73"/>
+      <c r="U25" s="73"/>
+      <c r="V25" s="73"/>
+      <c r="W25" s="73"/>
+      <c r="X25" s="73"/>
+      <c r="Y25" s="73"/>
+      <c r="Z25" s="73"/>
+      <c r="AA25" s="73"/>
+      <c r="AB25" s="73"/>
+    </row>
+    <row r="26" spans="1:28" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B26" s="83"/>
+      <c r="C26" s="83"/>
+      <c r="D26" s="83"/>
+      <c r="E26" s="83"/>
+      <c r="F26" s="83"/>
+      <c r="G26" s="83"/>
+      <c r="H26" s="83"/>
+      <c r="I26" s="83"/>
+      <c r="J26" s="83"/>
+      <c r="K26" s="83"/>
+      <c r="L26" s="83"/>
+      <c r="M26" s="83"/>
+      <c r="N26" s="83"/>
+      <c r="O26" s="83"/>
+      <c r="P26" s="83"/>
+      <c r="Q26" s="83"/>
+      <c r="R26" s="83"/>
+      <c r="S26" s="83"/>
+      <c r="T26" s="83"/>
+      <c r="U26" s="83"/>
+      <c r="V26" s="83"/>
+      <c r="W26" s="83"/>
+      <c r="X26" s="83"/>
+      <c r="Y26" s="83"/>
+      <c r="Z26" s="83"/>
+      <c r="AA26" s="83"/>
+      <c r="AB26" s="83"/>
+    </row>
+    <row r="27" spans="1:28" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="F27" s="65"/>
+      <c r="G27" s="99"/>
+    </row>
+    <row r="28" spans="1:28" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A28" s="85" t="s">
         <v>50</v>
       </c>
-      <c r="C22" s="80"/>
-      <c r="D22" s="80"/>
-      <c r="E22" s="80"/>
-    </row>
-    <row r="23" spans="1:28" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A23" s="88" t="s">
+      <c r="C28" s="80"/>
+      <c r="D28" s="80"/>
+      <c r="E28" s="80"/>
+    </row>
+    <row r="29" spans="1:28" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A29" s="88" t="s">
         <v>59</v>
       </c>
-      <c r="B23" s="65"/>
-      <c r="C23" s="65"/>
-      <c r="D23" s="65"/>
-      <c r="E23" s="65"/>
+      <c r="B29" s="65"/>
+      <c r="C29" s="65"/>
+      <c r="D29" s="65"/>
+      <c r="E29" s="65"/>
     </row>
   </sheetData>
   <phoneticPr fontId="3" type="noConversion"/>
@@ -2514,6 +2702,162 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr>
+    <pageSetUpPr fitToPage="1"/>
+  </sheetPr>
+  <dimension ref="A1:F9"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="18.625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="18.625" style="43"/>
+    <col min="2" max="6" width="18.625" style="91" customWidth="1"/>
+    <col min="7" max="16384" width="18.625" style="71"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="95" t="str">
+        <f>Content!A4 &amp; ": " &amp;Content!B4</f>
+        <v>eHS(S)D0033-03: Report on yearly PPP-KG claim transaction by school code (YYYY/YY)</v>
+      </c>
+      <c r="B1" s="90"/>
+      <c r="F1" s="92"/>
+    </row>
+    <row r="2" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="81"/>
+      <c r="B2" s="90"/>
+      <c r="F2" s="92"/>
+    </row>
+    <row r="3" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="40" t="s">
+        <v>28</v>
+      </c>
+      <c r="B3" s="90"/>
+      <c r="F3" s="92"/>
+    </row>
+    <row r="4" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="40"/>
+      <c r="B4" s="90"/>
+      <c r="F4" s="92"/>
+    </row>
+    <row r="5" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="81"/>
+      <c r="B5" s="105" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="96" t="s">
+        <v>69</v>
+      </c>
+      <c r="B6" s="93" t="s">
+        <v>70</v>
+      </c>
+      <c r="C6" s="93" t="s">
+        <v>71</v>
+      </c>
+      <c r="D6" s="93" t="s">
+        <v>56</v>
+      </c>
+      <c r="E6" s="94" t="s">
+        <v>55</v>
+      </c>
+      <c r="F6" s="94" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="81"/>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="3" type="noConversion"/>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup paperSize="9" scale="84" orientation="landscape" r:id="rId1"/>
+  <headerFooter alignWithMargins="0"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr>
+    <pageSetUpPr fitToPage="1"/>
+  </sheetPr>
+  <dimension ref="A1:F9"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="18.625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="18.625" style="43"/>
+    <col min="2" max="6" width="18.625" style="91" customWidth="1"/>
+    <col min="7" max="16384" width="18.625" style="71"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="95" t="str">
+        <f>Content!A4 &amp; ": " &amp;Content!B4</f>
+        <v>eHS(S)D0033-03: Report on yearly PPP-KG claim transaction by school code (YYYY/YY)</v>
+      </c>
+      <c r="B1" s="90"/>
+      <c r="F1" s="92"/>
+    </row>
+    <row r="2" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="81"/>
+      <c r="B2" s="90"/>
+      <c r="F2" s="92"/>
+    </row>
+    <row r="3" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="40" t="s">
+        <v>28</v>
+      </c>
+      <c r="B3" s="90"/>
+      <c r="F3" s="92"/>
+    </row>
+    <row r="4" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="40"/>
+      <c r="B4" s="90"/>
+      <c r="F4" s="92"/>
+    </row>
+    <row r="5" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="81"/>
+      <c r="B5" s="105" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="96" t="s">
+        <v>69</v>
+      </c>
+      <c r="B6" s="93" t="s">
+        <v>70</v>
+      </c>
+      <c r="C6" s="93" t="s">
+        <v>71</v>
+      </c>
+      <c r="D6" s="93" t="s">
+        <v>56</v>
+      </c>
+      <c r="E6" s="94" t="s">
+        <v>55</v>
+      </c>
+      <c r="F6" s="94" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="81"/>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="3" type="noConversion"/>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup paperSize="9" scale="84" orientation="landscape" r:id="rId1"/>
+  <headerFooter alignWithMargins="0"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
@@ -2673,7 +3017,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B45"/>
   <sheetViews>
@@ -2864,69 +3208,4 @@
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
   <headerFooter alignWithMargins="0"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D4"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="8.5" style="44" customWidth="1"/>
-    <col min="2" max="2" width="14.375" style="44" customWidth="1"/>
-    <col min="3" max="3" width="83.375" style="44" customWidth="1"/>
-    <col min="4" max="4" width="15.625" style="44" customWidth="1"/>
-    <col min="5" max="16384" width="9" style="44"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="11" t="s">
-        <v>33</v>
-      </c>
-      <c r="B1" s="1"/>
-      <c r="C1" s="1"/>
-      <c r="D1" s="1"/>
-    </row>
-    <row r="2" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="1"/>
-      <c r="B2" s="1"/>
-      <c r="C2" s="1"/>
-      <c r="D2" s="1"/>
-    </row>
-    <row r="3" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="2" t="s">
-        <v>29</v>
-      </c>
-      <c r="B3" s="2" t="s">
-        <v>30</v>
-      </c>
-      <c r="C3" s="2" t="s">
-        <v>31</v>
-      </c>
-      <c r="D3" s="2" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" ht="45" x14ac:dyDescent="0.25">
-      <c r="A4" s="88">
-        <v>1</v>
-      </c>
-      <c r="B4" s="88" t="s">
-        <v>84</v>
-      </c>
-      <c r="C4" s="100" t="s">
-        <v>74</v>
-      </c>
-      <c r="D4" s="104">
-        <v>43747</v>
-      </c>
-    </row>
-  </sheetData>
-  <phoneticPr fontId="3" type="noConversion"/>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
-  <headerFooter alignWithMargins="0"/>
-</worksheet>
 </file>
</xml_diff>

<commit_message>
20211007 INT21-0025	Fix DHC missing clear session
</commit_message>
<xml_diff>
--- a/EHS2019/EHS/ExcelGenerator/Template/eHSD0033-PPPKG Claim_Template.xlsx
+++ b/EHS2019/EHS/ExcelGenerator/Template/eHSD0033-PPPKG Claim_Template.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\ce5-fs01\ehs$\Development\InternalChangeControl\2020\CRE20-0XX (Gov SIV 2020_21)\Front-end (Phase 2)\ExcelGenerator\Template\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\ce5-fs01\ehs$\Development\InternalChangeControl\2021\INT21-0025 (Fix DHC missing clear session)\Front-end\ExcelGenerator\Template\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -17,18 +17,16 @@
     <sheet name="02-Age Group" sheetId="22" r:id="rId3"/>
     <sheet name="03-QIV" sheetId="28" r:id="rId4"/>
     <sheet name="03-LAIV" sheetId="29" r:id="rId5"/>
-    <sheet name="03-QIV (Govt)" sheetId="30" r:id="rId6"/>
-    <sheet name="03-LAIV (Govt)" sheetId="31" r:id="rId7"/>
-    <sheet name="04-Raw Data" sheetId="23" r:id="rId8"/>
-    <sheet name="Remark" sheetId="6" r:id="rId9"/>
-    <sheet name="Change History" sheetId="25" r:id="rId10"/>
+    <sheet name="04-Raw Data" sheetId="23" r:id="rId6"/>
+    <sheet name="Remark" sheetId="6" r:id="rId7"/>
+    <sheet name="Change History" sheetId="25" r:id="rId8"/>
   </sheets>
   <calcPr calcId="162913"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="311" uniqueCount="87">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="267" uniqueCount="87">
   <si>
     <t/>
   </si>
@@ -1149,87 +1147,6 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D5"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="8.5" style="44" customWidth="1"/>
-    <col min="2" max="2" width="14.375" style="44" customWidth="1"/>
-    <col min="3" max="3" width="84.875" style="44" customWidth="1"/>
-    <col min="4" max="4" width="15.625" style="44" customWidth="1"/>
-    <col min="5" max="16384" width="9" style="44"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="11" t="s">
-        <v>33</v>
-      </c>
-      <c r="B1" s="1"/>
-      <c r="C1" s="1"/>
-      <c r="D1" s="1"/>
-    </row>
-    <row r="2" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="1"/>
-      <c r="B2" s="1"/>
-      <c r="C2" s="1"/>
-      <c r="D2" s="1"/>
-    </row>
-    <row r="3" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="2" t="s">
-        <v>29</v>
-      </c>
-      <c r="B3" s="2" t="s">
-        <v>30</v>
-      </c>
-      <c r="C3" s="2" t="s">
-        <v>31</v>
-      </c>
-      <c r="D3" s="2" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A4" s="88">
-        <v>1</v>
-      </c>
-      <c r="B4" s="88" t="s">
-        <v>84</v>
-      </c>
-      <c r="C4" s="100" t="s">
-        <v>74</v>
-      </c>
-      <c r="D4" s="104">
-        <v>43747</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" ht="16.5" x14ac:dyDescent="0.25">
-      <c r="A5" s="88">
-        <v>2</v>
-      </c>
-      <c r="B5" s="88" t="s">
-        <v>85</v>
-      </c>
-      <c r="C5" s="100" t="s">
-        <v>86</v>
-      </c>
-      <c r="D5" s="104">
-        <v>44151</v>
-      </c>
-    </row>
-  </sheetData>
-  <phoneticPr fontId="3" type="noConversion"/>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
-  <headerFooter alignWithMargins="0"/>
-</worksheet>
-</file>
-
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
@@ -1940,7 +1857,7 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:AB29"/>
+  <dimension ref="A1:AB24"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -1953,7 +1870,7 @@
     <col min="5" max="16384" width="18.625" style="88"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" s="85" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:28" s="85" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="15" t="str">
         <f>Content!A3 &amp; ": " &amp;Content!B3</f>
         <v>eHS(S)D0033-02: Report on yearly PPP-KG claim transaction by age group and target group (YYYY/YY)</v>
@@ -1964,7 +1881,7 @@
       <c r="E1" s="101"/>
       <c r="F1" s="102"/>
     </row>
-    <row r="2" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:28" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="97"/>
       <c r="B2" s="81"/>
       <c r="C2" s="98"/>
@@ -1972,7 +1889,7 @@
       <c r="E2" s="98"/>
       <c r="F2" s="55"/>
     </row>
-    <row r="3" spans="1:9" s="85" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:28" s="85" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="57" t="s">
         <v>38</v>
       </c>
@@ -1982,10 +1899,10 @@
       <c r="E3" s="101"/>
       <c r="F3" s="102"/>
     </row>
-    <row r="4" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:28" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="80"/>
     </row>
-    <row r="5" spans="1:9" s="8" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:28" s="8" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="62" t="s">
         <v>60</v>
       </c>
@@ -1998,7 +1915,7 @@
       <c r="H5" s="85"/>
       <c r="I5" s="75"/>
     </row>
-    <row r="6" spans="1:9" s="49" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:28" s="49" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="82"/>
       <c r="B6" s="79"/>
       <c r="C6" s="65"/>
@@ -2008,7 +1925,7 @@
       <c r="H6" s="88"/>
       <c r="I6" s="65"/>
     </row>
-    <row r="7" spans="1:9" s="8" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:28" s="8" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="67" t="s">
         <v>25</v>
       </c>
@@ -2027,7 +1944,7 @@
       <c r="H7" s="85"/>
       <c r="I7" s="61"/>
     </row>
-    <row r="8" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:28" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="79" t="s">
         <v>39</v>
       </c>
@@ -2041,7 +1958,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="9" spans="1:9" s="49" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:28" s="49" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="82"/>
       <c r="B9" s="79"/>
       <c r="C9" s="65"/>
@@ -2051,7 +1968,7 @@
       <c r="H9" s="88"/>
       <c r="I9" s="65"/>
     </row>
-    <row r="10" spans="1:9" s="8" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:28" s="8" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="67" t="s">
         <v>25</v>
       </c>
@@ -2070,7 +1987,7 @@
       <c r="H10" s="85"/>
       <c r="I10" s="61"/>
     </row>
-    <row r="11" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:28" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="79" t="s">
         <v>39</v>
       </c>
@@ -2084,211 +2001,276 @@
         <v>39</v>
       </c>
     </row>
-    <row r="12" spans="1:9" s="49" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="82"/>
+    <row r="12" spans="1:28" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A12" s="79"/>
       <c r="B12" s="79"/>
-      <c r="C12" s="65"/>
-      <c r="D12" s="65"/>
-      <c r="F12" s="82"/>
-      <c r="G12" s="88"/>
-      <c r="H12" s="88"/>
-      <c r="I12" s="65"/>
-    </row>
-    <row r="13" spans="1:9" s="8" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="67" t="s">
-        <v>25</v>
-      </c>
-      <c r="B13" s="67" t="s">
-        <v>25</v>
-      </c>
-      <c r="C13" s="67" t="s">
-        <v>25</v>
-      </c>
-      <c r="D13" s="75" t="s">
-        <v>41</v>
-      </c>
-      <c r="E13" s="61"/>
-      <c r="F13" s="61"/>
-      <c r="G13" s="85"/>
-      <c r="H13" s="85"/>
-      <c r="I13" s="61"/>
-    </row>
-    <row r="14" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="79" t="s">
-        <v>39</v>
-      </c>
-      <c r="B14" s="79" t="s">
-        <v>26</v>
-      </c>
-      <c r="C14" s="79" t="s">
-        <v>26</v>
-      </c>
-      <c r="D14" s="79" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="15" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="79"/>
-      <c r="B15" s="79"/>
-      <c r="C15" s="79"/>
-      <c r="D15" s="79"/>
-      <c r="E15" s="79"/>
-    </row>
-    <row r="17" spans="1:28" s="85" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="74" t="s">
+      <c r="C12" s="79"/>
+      <c r="D12" s="79"/>
+      <c r="E12" s="79"/>
+    </row>
+    <row r="14" spans="1:28" s="85" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A14" s="74" t="s">
         <v>61</v>
       </c>
     </row>
-    <row r="18" spans="1:28" s="68" customFormat="1" ht="33" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B18" s="66" t="s">
+    <row r="15" spans="1:28" s="68" customFormat="1" ht="33" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B15" s="66" t="s">
         <v>37</v>
       </c>
-      <c r="C18" s="75" t="s">
+      <c r="C15" s="75" t="s">
         <v>37</v>
       </c>
-      <c r="D18" s="75" t="s">
+      <c r="D15" s="75" t="s">
         <v>37</v>
       </c>
-      <c r="E18" s="75" t="s">
+      <c r="E15" s="75" t="s">
         <v>48</v>
       </c>
-      <c r="F18" s="75" t="s">
+      <c r="F15" s="75" t="s">
         <v>48</v>
       </c>
-      <c r="G18" s="75" t="s">
+      <c r="G15" s="75" t="s">
         <v>48</v>
       </c>
-      <c r="H18" s="68" t="s">
+      <c r="H15" s="68" t="s">
         <v>49</v>
       </c>
-      <c r="I18" s="68" t="s">
+      <c r="I15" s="68" t="s">
         <v>68</v>
       </c>
-      <c r="J18" s="77" t="s">
+      <c r="J15" s="77" t="s">
         <v>51</v>
       </c>
-      <c r="P18" s="69"/>
-      <c r="Q18" s="69"/>
-      <c r="R18" s="69"/>
-      <c r="S18" s="69"/>
-      <c r="T18" s="69"/>
-      <c r="U18" s="69"/>
-      <c r="V18" s="75"/>
-      <c r="W18" s="75"/>
-      <c r="X18" s="75"/>
-      <c r="Y18" s="75"/>
-      <c r="Z18" s="75"/>
-      <c r="AA18" s="75"/>
-      <c r="AB18" s="77"/>
-    </row>
-    <row r="19" spans="1:28" s="84" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="68"/>
-      <c r="B19" s="84" t="s">
+      <c r="P15" s="69"/>
+      <c r="Q15" s="69"/>
+      <c r="R15" s="69"/>
+      <c r="S15" s="69"/>
+      <c r="T15" s="69"/>
+      <c r="U15" s="69"/>
+      <c r="V15" s="75"/>
+      <c r="W15" s="75"/>
+      <c r="X15" s="75"/>
+      <c r="Y15" s="75"/>
+      <c r="Z15" s="75"/>
+      <c r="AA15" s="75"/>
+      <c r="AB15" s="77"/>
+    </row>
+    <row r="16" spans="1:28" s="84" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A16" s="68"/>
+      <c r="B16" s="84" t="s">
         <v>42</v>
       </c>
-      <c r="C19" s="84" t="s">
+      <c r="C16" s="84" t="s">
         <v>43</v>
       </c>
-      <c r="D19" s="84" t="s">
+      <c r="D16" s="84" t="s">
         <v>44</v>
       </c>
-      <c r="E19" s="84" t="s">
+      <c r="E16" s="84" t="s">
         <v>45</v>
       </c>
-      <c r="F19" s="84" t="s">
+      <c r="F16" s="84" t="s">
         <v>46</v>
       </c>
-      <c r="G19" s="84" t="s">
+      <c r="G16" s="84" t="s">
         <v>47</v>
       </c>
-      <c r="H19" s="84" t="s">
+      <c r="H16" s="84" t="s">
         <v>47</v>
       </c>
-      <c r="I19" s="84" t="s">
+      <c r="I16" s="84" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="20" spans="1:28" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="49" t="s">
+    <row r="17" spans="1:28" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A17" s="49" t="s">
         <v>40</v>
       </c>
-      <c r="B20" s="83" t="s">
+      <c r="B17" s="83" t="s">
         <v>40</v>
       </c>
-      <c r="C20" s="83" t="s">
+      <c r="C17" s="83" t="s">
         <v>40</v>
       </c>
-      <c r="D20" s="83" t="s">
+      <c r="D17" s="83" t="s">
         <v>40</v>
       </c>
-      <c r="E20" s="83" t="s">
+      <c r="E17" s="83" t="s">
         <v>40</v>
       </c>
-      <c r="F20" s="83" t="s">
+      <c r="F17" s="83" t="s">
         <v>40</v>
       </c>
-      <c r="G20" s="83" t="s">
+      <c r="G17" s="83" t="s">
         <v>40</v>
       </c>
-      <c r="H20" s="83" t="s">
+      <c r="H17" s="83" t="s">
         <v>40</v>
       </c>
-      <c r="I20" s="83" t="s">
+      <c r="I17" s="83" t="s">
         <v>40</v>
       </c>
-      <c r="J20" s="83" t="s">
+      <c r="J17" s="83" t="s">
         <v>40</v>
       </c>
-      <c r="K20" s="83"/>
-      <c r="L20" s="83"/>
-      <c r="M20" s="83"/>
-      <c r="N20" s="83"/>
-      <c r="O20" s="83"/>
-      <c r="P20" s="83"/>
-      <c r="Q20" s="83"/>
-      <c r="R20" s="83"/>
-      <c r="S20" s="83"/>
-      <c r="T20" s="83"/>
-      <c r="U20" s="83"/>
-      <c r="V20" s="83"/>
-      <c r="W20" s="83"/>
-      <c r="X20" s="83"/>
-      <c r="Y20" s="83"/>
-      <c r="Z20" s="83"/>
-      <c r="AA20" s="83"/>
-      <c r="AB20" s="83"/>
+      <c r="K17" s="83"/>
+      <c r="L17" s="83"/>
+      <c r="M17" s="83"/>
+      <c r="N17" s="83"/>
+      <c r="O17" s="83"/>
+      <c r="P17" s="83"/>
+      <c r="Q17" s="83"/>
+      <c r="R17" s="83"/>
+      <c r="S17" s="83"/>
+      <c r="T17" s="83"/>
+      <c r="U17" s="83"/>
+      <c r="V17" s="83"/>
+      <c r="W17" s="83"/>
+      <c r="X17" s="83"/>
+      <c r="Y17" s="83"/>
+      <c r="Z17" s="83"/>
+      <c r="AA17" s="83"/>
+      <c r="AB17" s="83"/>
+    </row>
+    <row r="18" spans="1:28" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A18" s="49" t="s">
+        <v>26</v>
+      </c>
+      <c r="B18" s="83" t="s">
+        <v>26</v>
+      </c>
+      <c r="C18" s="83" t="s">
+        <v>26</v>
+      </c>
+      <c r="D18" s="83" t="s">
+        <v>26</v>
+      </c>
+      <c r="E18" s="83" t="s">
+        <v>26</v>
+      </c>
+      <c r="F18" s="83" t="s">
+        <v>26</v>
+      </c>
+      <c r="G18" s="83" t="s">
+        <v>26</v>
+      </c>
+      <c r="H18" s="83" t="s">
+        <v>26</v>
+      </c>
+      <c r="I18" s="83" t="s">
+        <v>26</v>
+      </c>
+      <c r="J18" s="83" t="s">
+        <v>26</v>
+      </c>
+      <c r="K18" s="83"/>
+      <c r="L18" s="83"/>
+      <c r="M18" s="83"/>
+      <c r="N18" s="83"/>
+      <c r="O18" s="83"/>
+      <c r="P18" s="83"/>
+      <c r="Q18" s="83"/>
+      <c r="R18" s="83"/>
+      <c r="S18" s="83"/>
+      <c r="T18" s="83"/>
+      <c r="U18" s="83"/>
+      <c r="V18" s="83"/>
+      <c r="W18" s="83"/>
+      <c r="X18" s="83"/>
+      <c r="Y18" s="83"/>
+      <c r="Z18" s="83"/>
+      <c r="AA18" s="83"/>
+      <c r="AB18" s="83"/>
+    </row>
+    <row r="19" spans="1:28" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B19" s="83"/>
+      <c r="C19" s="83"/>
+      <c r="D19" s="83"/>
+      <c r="E19" s="83"/>
+      <c r="F19" s="83"/>
+      <c r="G19" s="83"/>
+      <c r="H19" s="83"/>
+      <c r="I19" s="83"/>
+      <c r="J19" s="83"/>
+      <c r="K19" s="83"/>
+      <c r="L19" s="83"/>
+      <c r="M19" s="83"/>
+      <c r="N19" s="83"/>
+      <c r="O19" s="83"/>
+      <c r="P19" s="83"/>
+      <c r="Q19" s="83"/>
+      <c r="R19" s="83"/>
+      <c r="S19" s="83"/>
+      <c r="T19" s="83"/>
+      <c r="U19" s="83"/>
+      <c r="V19" s="83"/>
+      <c r="W19" s="83"/>
+      <c r="X19" s="83"/>
+      <c r="Y19" s="83"/>
+      <c r="Z19" s="83"/>
+      <c r="AA19" s="83"/>
+      <c r="AB19" s="83"/>
+    </row>
+    <row r="20" spans="1:28" s="85" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A20" s="85" t="s">
+        <v>83</v>
+      </c>
+      <c r="B20" s="73" t="s">
+        <v>40</v>
+      </c>
+      <c r="C20" s="73" t="s">
+        <v>40</v>
+      </c>
+      <c r="D20" s="73" t="s">
+        <v>40</v>
+      </c>
+      <c r="E20" s="73" t="s">
+        <v>40</v>
+      </c>
+      <c r="F20" s="73" t="s">
+        <v>40</v>
+      </c>
+      <c r="G20" s="73" t="s">
+        <v>40</v>
+      </c>
+      <c r="H20" s="73" t="s">
+        <v>40</v>
+      </c>
+      <c r="I20" s="73" t="s">
+        <v>40</v>
+      </c>
+      <c r="J20" s="73" t="s">
+        <v>40</v>
+      </c>
+      <c r="K20" s="73"/>
+      <c r="L20" s="73"/>
+      <c r="M20" s="73"/>
+      <c r="N20" s="73"/>
+      <c r="O20" s="73"/>
+      <c r="P20" s="73"/>
+      <c r="Q20" s="73"/>
+      <c r="R20" s="73"/>
+      <c r="S20" s="73"/>
+      <c r="T20" s="73"/>
+      <c r="U20" s="73"/>
+      <c r="V20" s="73"/>
+      <c r="W20" s="73"/>
+      <c r="X20" s="73"/>
+      <c r="Y20" s="73"/>
+      <c r="Z20" s="73"/>
+      <c r="AA20" s="73"/>
+      <c r="AB20" s="73"/>
     </row>
     <row r="21" spans="1:28" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A21" s="49" t="s">
-        <v>26</v>
-      </c>
-      <c r="B21" s="83" t="s">
-        <v>26</v>
-      </c>
-      <c r="C21" s="83" t="s">
-        <v>26</v>
-      </c>
-      <c r="D21" s="83" t="s">
-        <v>26</v>
-      </c>
-      <c r="E21" s="83" t="s">
-        <v>26</v>
-      </c>
-      <c r="F21" s="83" t="s">
-        <v>26</v>
-      </c>
-      <c r="G21" s="83" t="s">
-        <v>26</v>
-      </c>
-      <c r="H21" s="83" t="s">
-        <v>26</v>
-      </c>
-      <c r="I21" s="83" t="s">
-        <v>26</v>
-      </c>
-      <c r="J21" s="83" t="s">
-        <v>26</v>
-      </c>
+      <c r="B21" s="83"/>
+      <c r="C21" s="83"/>
+      <c r="D21" s="83"/>
+      <c r="E21" s="83"/>
+      <c r="F21" s="83"/>
+      <c r="G21" s="83"/>
+      <c r="H21" s="83"/>
+      <c r="I21" s="83"/>
+      <c r="J21" s="83"/>
       <c r="K21" s="83"/>
       <c r="L21" s="83"/>
       <c r="M21" s="83"/>
@@ -2309,233 +2291,25 @@
       <c r="AB21" s="83"/>
     </row>
     <row r="22" spans="1:28" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A22" s="49" t="s">
-        <v>39</v>
-      </c>
-      <c r="B22" s="83" t="s">
-        <v>39</v>
-      </c>
-      <c r="C22" s="83" t="s">
-        <v>39</v>
-      </c>
-      <c r="D22" s="83" t="s">
-        <v>39</v>
-      </c>
-      <c r="E22" s="83" t="s">
-        <v>39</v>
-      </c>
-      <c r="F22" s="83" t="s">
-        <v>39</v>
-      </c>
-      <c r="G22" s="83" t="s">
-        <v>39</v>
-      </c>
-      <c r="H22" s="83" t="s">
-        <v>39</v>
-      </c>
-      <c r="I22" s="83" t="s">
-        <v>39</v>
-      </c>
-      <c r="J22" s="83" t="s">
-        <v>39</v>
-      </c>
-      <c r="K22" s="83"/>
-      <c r="L22" s="83"/>
-      <c r="M22" s="83"/>
-      <c r="N22" s="83"/>
-      <c r="O22" s="83"/>
-      <c r="P22" s="83"/>
-      <c r="Q22" s="83"/>
-      <c r="R22" s="83"/>
-      <c r="S22" s="83"/>
-      <c r="T22" s="83"/>
-      <c r="U22" s="83"/>
-      <c r="V22" s="83"/>
-      <c r="W22" s="83"/>
-      <c r="X22" s="83"/>
-      <c r="Y22" s="83"/>
-      <c r="Z22" s="83"/>
-      <c r="AA22" s="83"/>
-      <c r="AB22" s="83"/>
+      <c r="F22" s="65"/>
+      <c r="G22" s="99"/>
     </row>
     <row r="23" spans="1:28" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A23" s="49" t="s">
-        <v>26</v>
-      </c>
-      <c r="B23" s="83" t="s">
-        <v>26</v>
-      </c>
-      <c r="C23" s="83" t="s">
-        <v>26</v>
-      </c>
-      <c r="D23" s="83" t="s">
-        <v>26</v>
-      </c>
-      <c r="E23" s="83" t="s">
-        <v>26</v>
-      </c>
-      <c r="F23" s="83" t="s">
-        <v>26</v>
-      </c>
-      <c r="G23" s="83" t="s">
-        <v>26</v>
-      </c>
-      <c r="H23" s="83" t="s">
-        <v>26</v>
-      </c>
-      <c r="I23" s="83" t="s">
-        <v>26</v>
-      </c>
-      <c r="J23" s="83" t="s">
-        <v>26</v>
-      </c>
-      <c r="K23" s="83"/>
-      <c r="L23" s="83"/>
-      <c r="M23" s="83"/>
-      <c r="N23" s="83"/>
-      <c r="O23" s="83"/>
-      <c r="P23" s="83"/>
-      <c r="Q23" s="83"/>
-      <c r="R23" s="83"/>
-      <c r="S23" s="83"/>
-      <c r="T23" s="83"/>
-      <c r="U23" s="83"/>
-      <c r="V23" s="83"/>
-      <c r="W23" s="83"/>
-      <c r="X23" s="83"/>
-      <c r="Y23" s="83"/>
-      <c r="Z23" s="83"/>
-      <c r="AA23" s="83"/>
-      <c r="AB23" s="83"/>
+      <c r="A23" s="85" t="s">
+        <v>50</v>
+      </c>
+      <c r="C23" s="80"/>
+      <c r="D23" s="80"/>
+      <c r="E23" s="80"/>
     </row>
     <row r="24" spans="1:28" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B24" s="83"/>
-      <c r="C24" s="83"/>
-      <c r="D24" s="83"/>
-      <c r="E24" s="83"/>
-      <c r="F24" s="83"/>
-      <c r="G24" s="83"/>
-      <c r="H24" s="83"/>
-      <c r="I24" s="83"/>
-      <c r="J24" s="83"/>
-      <c r="K24" s="83"/>
-      <c r="L24" s="83"/>
-      <c r="M24" s="83"/>
-      <c r="N24" s="83"/>
-      <c r="O24" s="83"/>
-      <c r="P24" s="83"/>
-      <c r="Q24" s="83"/>
-      <c r="R24" s="83"/>
-      <c r="S24" s="83"/>
-      <c r="T24" s="83"/>
-      <c r="U24" s="83"/>
-      <c r="V24" s="83"/>
-      <c r="W24" s="83"/>
-      <c r="X24" s="83"/>
-      <c r="Y24" s="83"/>
-      <c r="Z24" s="83"/>
-      <c r="AA24" s="83"/>
-      <c r="AB24" s="83"/>
-    </row>
-    <row r="25" spans="1:28" s="85" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A25" s="85" t="s">
-        <v>83</v>
-      </c>
-      <c r="B25" s="73" t="s">
-        <v>40</v>
-      </c>
-      <c r="C25" s="73" t="s">
-        <v>40</v>
-      </c>
-      <c r="D25" s="73" t="s">
-        <v>40</v>
-      </c>
-      <c r="E25" s="73" t="s">
-        <v>40</v>
-      </c>
-      <c r="F25" s="73" t="s">
-        <v>40</v>
-      </c>
-      <c r="G25" s="73" t="s">
-        <v>40</v>
-      </c>
-      <c r="H25" s="73" t="s">
-        <v>40</v>
-      </c>
-      <c r="I25" s="73" t="s">
-        <v>40</v>
-      </c>
-      <c r="J25" s="73" t="s">
-        <v>40</v>
-      </c>
-      <c r="K25" s="73"/>
-      <c r="L25" s="73"/>
-      <c r="M25" s="73"/>
-      <c r="N25" s="73"/>
-      <c r="O25" s="73"/>
-      <c r="P25" s="73"/>
-      <c r="Q25" s="73"/>
-      <c r="R25" s="73"/>
-      <c r="S25" s="73"/>
-      <c r="T25" s="73"/>
-      <c r="U25" s="73"/>
-      <c r="V25" s="73"/>
-      <c r="W25" s="73"/>
-      <c r="X25" s="73"/>
-      <c r="Y25" s="73"/>
-      <c r="Z25" s="73"/>
-      <c r="AA25" s="73"/>
-      <c r="AB25" s="73"/>
-    </row>
-    <row r="26" spans="1:28" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B26" s="83"/>
-      <c r="C26" s="83"/>
-      <c r="D26" s="83"/>
-      <c r="E26" s="83"/>
-      <c r="F26" s="83"/>
-      <c r="G26" s="83"/>
-      <c r="H26" s="83"/>
-      <c r="I26" s="83"/>
-      <c r="J26" s="83"/>
-      <c r="K26" s="83"/>
-      <c r="L26" s="83"/>
-      <c r="M26" s="83"/>
-      <c r="N26" s="83"/>
-      <c r="O26" s="83"/>
-      <c r="P26" s="83"/>
-      <c r="Q26" s="83"/>
-      <c r="R26" s="83"/>
-      <c r="S26" s="83"/>
-      <c r="T26" s="83"/>
-      <c r="U26" s="83"/>
-      <c r="V26" s="83"/>
-      <c r="W26" s="83"/>
-      <c r="X26" s="83"/>
-      <c r="Y26" s="83"/>
-      <c r="Z26" s="83"/>
-      <c r="AA26" s="83"/>
-      <c r="AB26" s="83"/>
-    </row>
-    <row r="27" spans="1:28" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="F27" s="65"/>
-      <c r="G27" s="99"/>
-    </row>
-    <row r="28" spans="1:28" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A28" s="85" t="s">
-        <v>50</v>
-      </c>
-      <c r="C28" s="80"/>
-      <c r="D28" s="80"/>
-      <c r="E28" s="80"/>
-    </row>
-    <row r="29" spans="1:28" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A29" s="88" t="s">
+      <c r="A24" s="88" t="s">
         <v>59</v>
       </c>
-      <c r="B29" s="65"/>
-      <c r="C29" s="65"/>
-      <c r="D29" s="65"/>
-      <c r="E29" s="65"/>
+      <c r="B24" s="65"/>
+      <c r="C24" s="65"/>
+      <c r="D24" s="65"/>
+      <c r="E24" s="65"/>
     </row>
   </sheetData>
   <phoneticPr fontId="3" type="noConversion"/>
@@ -2702,162 +2476,6 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <sheetPr>
-    <pageSetUpPr fitToPage="1"/>
-  </sheetPr>
-  <dimension ref="A1:F9"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultColWidth="18.625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="18.625" style="43"/>
-    <col min="2" max="6" width="18.625" style="91" customWidth="1"/>
-    <col min="7" max="16384" width="18.625" style="71"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="95" t="str">
-        <f>Content!A4 &amp; ": " &amp;Content!B4</f>
-        <v>eHS(S)D0033-03: Report on yearly PPP-KG claim transaction by school code (YYYY/YY)</v>
-      </c>
-      <c r="B1" s="90"/>
-      <c r="F1" s="92"/>
-    </row>
-    <row r="2" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="81"/>
-      <c r="B2" s="90"/>
-      <c r="F2" s="92"/>
-    </row>
-    <row r="3" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="40" t="s">
-        <v>28</v>
-      </c>
-      <c r="B3" s="90"/>
-      <c r="F3" s="92"/>
-    </row>
-    <row r="4" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="40"/>
-      <c r="B4" s="90"/>
-      <c r="F4" s="92"/>
-    </row>
-    <row r="5" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="81"/>
-      <c r="B5" s="105" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="96" t="s">
-        <v>69</v>
-      </c>
-      <c r="B6" s="93" t="s">
-        <v>70</v>
-      </c>
-      <c r="C6" s="93" t="s">
-        <v>71</v>
-      </c>
-      <c r="D6" s="93" t="s">
-        <v>56</v>
-      </c>
-      <c r="E6" s="94" t="s">
-        <v>55</v>
-      </c>
-      <c r="F6" s="94" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="9" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="81"/>
-    </row>
-  </sheetData>
-  <phoneticPr fontId="3" type="noConversion"/>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <pageSetup paperSize="9" scale="84" orientation="landscape" r:id="rId1"/>
-  <headerFooter alignWithMargins="0"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <sheetPr>
-    <pageSetUpPr fitToPage="1"/>
-  </sheetPr>
-  <dimension ref="A1:F9"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultColWidth="18.625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="18.625" style="43"/>
-    <col min="2" max="6" width="18.625" style="91" customWidth="1"/>
-    <col min="7" max="16384" width="18.625" style="71"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="95" t="str">
-        <f>Content!A4 &amp; ": " &amp;Content!B4</f>
-        <v>eHS(S)D0033-03: Report on yearly PPP-KG claim transaction by school code (YYYY/YY)</v>
-      </c>
-      <c r="B1" s="90"/>
-      <c r="F1" s="92"/>
-    </row>
-    <row r="2" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="81"/>
-      <c r="B2" s="90"/>
-      <c r="F2" s="92"/>
-    </row>
-    <row r="3" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="40" t="s">
-        <v>28</v>
-      </c>
-      <c r="B3" s="90"/>
-      <c r="F3" s="92"/>
-    </row>
-    <row r="4" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="40"/>
-      <c r="B4" s="90"/>
-      <c r="F4" s="92"/>
-    </row>
-    <row r="5" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="81"/>
-      <c r="B5" s="105" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="96" t="s">
-        <v>69</v>
-      </c>
-      <c r="B6" s="93" t="s">
-        <v>70</v>
-      </c>
-      <c r="C6" s="93" t="s">
-        <v>71</v>
-      </c>
-      <c r="D6" s="93" t="s">
-        <v>56</v>
-      </c>
-      <c r="E6" s="94" t="s">
-        <v>55</v>
-      </c>
-      <c r="F6" s="94" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="9" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="81"/>
-    </row>
-  </sheetData>
-  <phoneticPr fontId="3" type="noConversion"/>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <pageSetup paperSize="9" scale="84" orientation="landscape" r:id="rId1"/>
-  <headerFooter alignWithMargins="0"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
@@ -3017,7 +2635,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B45"/>
   <sheetViews>
@@ -3208,4 +2826,83 @@
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
   <headerFooter alignWithMargins="0"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:D5"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="8.5" style="44" customWidth="1"/>
+    <col min="2" max="2" width="14.375" style="44" customWidth="1"/>
+    <col min="3" max="3" width="84.875" style="44" customWidth="1"/>
+    <col min="4" max="4" width="15.625" style="44" customWidth="1"/>
+    <col min="5" max="16384" width="9" style="44"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="11" t="s">
+        <v>33</v>
+      </c>
+      <c r="B1" s="1"/>
+      <c r="C1" s="1"/>
+      <c r="D1" s="1"/>
+    </row>
+    <row r="2" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="1"/>
+      <c r="B2" s="1"/>
+      <c r="C2" s="1"/>
+      <c r="D2" s="1"/>
+    </row>
+    <row r="3" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="D3" s="2" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A4" s="88">
+        <v>1</v>
+      </c>
+      <c r="B4" s="88" t="s">
+        <v>84</v>
+      </c>
+      <c r="C4" s="100" t="s">
+        <v>74</v>
+      </c>
+      <c r="D4" s="104">
+        <v>43747</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="A5" s="88">
+        <v>2</v>
+      </c>
+      <c r="B5" s="88" t="s">
+        <v>85</v>
+      </c>
+      <c r="C5" s="100" t="s">
+        <v>86</v>
+      </c>
+      <c r="D5" s="104">
+        <v>44151</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="3" type="noConversion"/>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+  <headerFooter alignWithMargins="0"/>
+</worksheet>
 </file>
</xml_diff>